<commit_message>
added face recognizers, managed to convert labels into strings
</commit_message>
<xml_diff>
--- a/Diagrams and Spreedsheets/SVMlinearkernel.xlsx
+++ b/Diagrams and Spreedsheets/SVMlinearkernel.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t xml:space="preserve">Trial Number</t>
   </si>
@@ -29,6 +29,9 @@
   </si>
   <si>
     <t xml:space="preserve">Cross Validation Scores</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dasf</t>
   </si>
 </sst>
 </file>
@@ -263,6 +266,7 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -406,6 +410,7 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -522,11 +527,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="30379772"/>
-        <c:axId val="32758956"/>
+        <c:axId val="71884075"/>
+        <c:axId val="7802865"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="30379772"/>
+        <c:axId val="71884075"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -576,14 +581,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="32758956"/>
+        <c:crossAx val="7802865"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="32758956"/>
+        <c:axId val="7802865"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -620,7 +625,7 @@
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -642,7 +647,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="30379772"/>
+        <c:crossAx val="71884075"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -701,9 +706,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>300600</xdr:colOff>
+      <xdr:colOff>300240</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>6480</xdr:rowOff>
+      <xdr:rowOff>6120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -711,8 +716,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="3627720" y="195840"/>
-        <a:ext cx="5759640" cy="3239640"/>
+        <a:off x="3630960" y="195840"/>
+        <a:ext cx="5765400" cy="3239280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -733,12 +738,12 @@
   <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R12" activeCellId="0" sqref="R12"/>
+      <selection pane="topLeft" activeCell="B33" activeCellId="0" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1083,9 +1088,8 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="0" t="n">
-        <f aca="false">AVERAGE(B1:B31)</f>
-        <v>75.9333333333334</v>
+      <c r="B32" s="0" t="s">
+        <v>3</v>
       </c>
       <c r="C32" s="0" t="n">
         <f aca="false">AVERAGE(C1:C31)</f>
@@ -1094,8 +1098,7 @@
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="0" t="n">
-        <f aca="false">STDEV(B1:B31)</f>
-        <v>2.76117582816144</v>
+        <v>3</v>
       </c>
       <c r="C33" s="0" t="n">
         <f aca="false">STDEV(C1:C31)</f>

</xml_diff>